<commit_message>
Cell model validation results
</commit_message>
<xml_diff>
--- a/morphology-data/morphology-metrics-and-sources.xlsx
+++ b/morphology-data/morphology-metrics-and-sources.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="178">
   <si>
     <t>Granule Cell Apical Dendrite Average Bifurcation Angle Local</t>
   </si>
@@ -561,6 +561,9 @@
   </si>
   <si>
     <t>Burton and Urban (2014), Burton et al. (2017), Fukunaga et al. (2012)</t>
+  </si>
+  <si>
+    <t>Migliore2007 MC</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -660,6 +663,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2983,9 +2987,9 @@
         <v>329.05 ± 234.91 (61)</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>159</v>
+    <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>177</v>
       </c>
       <c r="B48" s="10">
         <v>0.47144692173716102</v>

</xml_diff>